<commit_message>
Added bug from issue 63549 - tensorflow
</commit_message>
<xml_diff>
--- a/bug_dataset.xlsx
+++ b/bug_dataset.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>Issue #</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>fx_codegen_and_compile(),run_node()</t>
+  </si>
+  <si>
+    <t>Inconsistency in XLA Cotionmpila with Operand Order Swap in tf.add with Specific Operators on GPU</t>
+  </si>
+  <si>
+    <t>https://github.com/openxla/xla/tree/main/xla/service/gpu/ir_emission_utils.cc</t>
+  </si>
+  <si>
+    <t>FindTransposeHero, transpose</t>
   </si>
 </sst>
 </file>
@@ -586,6 +595,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="3" max="3" width="76.38"/>
     <col customWidth="1" min="7" max="7" width="16.5"/>
   </cols>
   <sheetData>
@@ -612,12 +622,40 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>63549.0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>7899.0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Z1">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Force pushed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="B2"/>
+    <hyperlink r:id="rId3" ref="F2"/>
+  </hyperlinks>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added details of all inspected tensorflow bugs
</commit_message>
<xml_diff>
--- a/bug_dataset.xlsx
+++ b/bug_dataset.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
   <si>
     <t>Issue #</t>
   </si>
@@ -81,6 +81,96 @@
     <t>fx_codegen_and_compile(),run_node()</t>
   </si>
   <si>
+    <t>Filter:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is:issue is:closed created:2023-12-01..2024-03-27 label:type:bug </t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>tf.raw_ops.UnravelIndex can leads to eigen assertion failure</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>tensorflow/core/kernels/unravel_index_op.cc</t>
+  </si>
+  <si>
+    <t>UnravelIndexOp.Compute()</t>
+  </si>
+  <si>
+    <t>Did not reproduce: general operation specific bug</t>
+  </si>
+  <si>
+    <t>tf.raw_ops.Substr can lead to eigen assertion failure</t>
+  </si>
+  <si>
+    <t>tensorflow/core/kernels/substr_op.cc</t>
+  </si>
+  <si>
+    <t>SubstrOp.Compute()</t>
+  </si>
+  <si>
+    <t>Confusing result of tf.argsort/argmax/argmin/ given a boolean axis</t>
+  </si>
+  <si>
+    <t>tensorflow/python/ops/math_ops.py</t>
+  </si>
+  <si>
+    <t>argmax_v2()</t>
+  </si>
+  <si>
+    <t>Unit test failures with Python 3.12 and gcc</t>
+  </si>
+  <si>
+    <t>tensorflow/python/client/tf_session_wrapper.cc</t>
+  </si>
+  <si>
+    <t>PyGraphData.Clear()</t>
+  </si>
+  <si>
+    <t>Did not reproduce: data structure specific bug</t>
+  </si>
+  <si>
+    <t>tf.raw_ops.DrawBoundingBoxesV2 aborts with inappropriate input</t>
+  </si>
+  <si>
+    <t>tensorflow/core/kernels/image/draw_bounding_box_op.cc</t>
+  </si>
+  <si>
+    <t>DrawBoundingBoxesOp.Compute()</t>
+  </si>
+  <si>
+    <t>tf.raw_ops.RecordInput aborts with negative batch_size</t>
+  </si>
+  <si>
+    <t>tensorflow/core/kernels/record_input_op.cc</t>
+  </si>
+  <si>
+    <t>RecordInputOp.GETATTR()</t>
+  </si>
+  <si>
+    <t>remapper_test fails on AARCH64 with --config=mkl_aarch64_threadpool</t>
+  </si>
+  <si>
+    <t>tensorflow/core/grappler/optimizers/mkl_remapper_test.cc,tensorflow/core/grappler/optimizers/remapper_test.cc</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Did not reproduce: fixing tests</t>
+  </si>
+  <si>
+    <t>mkl_remapper_test fails with TF_ENABLE_ONEDNN_OPTS=1</t>
+  </si>
+  <si>
+    <t>tensorflow/core/grappler/optimizers/mkl_remapper_test.c,tensorflow/core/grappler/optimizers/remapper_test.cc</t>
+  </si>
+  <si>
     <t>Inconsistency in XLA Cotionmpila with Operand Order Swap in tf.add with Specific Operators on GPU</t>
   </si>
   <si>
@@ -88,6 +178,9 @@
   </si>
   <si>
     <t>FindTransposeHero, transpose</t>
+  </si>
+  <si>
+    <t>Reproduced: bug originates from the XLA compiler (not tensorflow repo)</t>
   </si>
 </sst>
 </file>
@@ -125,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -135,17 +228,28 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF4C7C3"/>
           <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
       <border/>
@@ -420,6 +524,25 @@
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="2">
@@ -443,6 +566,25 @@
       <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="2">
@@ -466,11 +608,35 @@
       <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Z1000">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Force pushed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:Z1000">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula> $D1 = "YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -545,6 +711,25 @@
       <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="2">
@@ -568,11 +753,35 @@
       <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Z1">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Force pushed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:Z1000">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula> $D1 = "YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -596,66 +805,336 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="3" max="3" width="76.38"/>
-    <col customWidth="1" min="7" max="7" width="16.5"/>
+    <col customWidth="1" min="7" max="7" width="24.38"/>
+    <col customWidth="1" min="8" max="8" width="47.75"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>63549.0</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>63037.0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>63092.0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>63036.0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>63091.0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>63031.0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>63050.0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>63012.0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>63083.0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>62981.0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>63105.0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>62977.0</v>
+      </c>
+      <c r="B8" s="2">
+        <v>62990.0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>62882.0</v>
+      </c>
+      <c r="B9" s="2">
+        <v>62897.0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>62835.0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>62876.0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>62549.0</v>
+      </c>
+      <c r="B11" s="2">
         <v>7899.0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Z1">
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:Z2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Force pushed"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A1:Z1001">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula> $D1 = "YES"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="F2"/>
+    <hyperlink r:id="rId1" ref="A3"/>
+    <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
+    <hyperlink r:id="rId4" ref="B4"/>
+    <hyperlink r:id="rId5" ref="A5"/>
+    <hyperlink r:id="rId6" ref="B5"/>
+    <hyperlink r:id="rId7" ref="A6"/>
+    <hyperlink r:id="rId8" ref="B6"/>
+    <hyperlink r:id="rId9" ref="A7"/>
+    <hyperlink r:id="rId10" ref="B7"/>
+    <hyperlink r:id="rId11" ref="A8"/>
+    <hyperlink r:id="rId12" ref="B8"/>
+    <hyperlink r:id="rId13" ref="A9"/>
+    <hyperlink r:id="rId14" ref="B9"/>
+    <hyperlink r:id="rId15" ref="A10"/>
+    <hyperlink r:id="rId16" ref="B10"/>
+    <hyperlink r:id="rId17" ref="A11"/>
+    <hyperlink r:id="rId18" ref="B11"/>
+    <hyperlink r:id="rId19" ref="F11"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated bug details from jax and pytorch libraries
</commit_message>
<xml_diff>
--- a/bug_dataset.xlsx
+++ b/bug_dataset.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="105">
+  <si>
+    <t>Filter:</t>
+  </si>
+  <si>
+    <t>is:issue is:closed created:2023-10-20..2024-03-27 label:bug</t>
+  </si>
   <si>
     <t>Issue #</t>
   </si>
@@ -36,6 +42,42 @@
     <t>Buggy Function(s)</t>
   </si>
   <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>grad(jit(f)) can fail when an output which is a forwarded input precedes an output which is also a residual</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Did not attempt</t>
+  </si>
+  <si>
+    <t>MLIRError raised when using jax.lax.shift_right_logical in pallas</t>
+  </si>
+  <si>
+    <t>jax.experimental.attrs: Spurious "AssertionError: a jaxpr variable must be created only once per tracer"</t>
+  </si>
+  <si>
+    <t>Executing genrule @tsl//tsl/cuda:cudnn_stub_gen failed</t>
+  </si>
+  <si>
+    <t>jax.vmap(jax.pure_callback(...), in_axes=1) is broken</t>
+  </si>
+  <si>
+    <t>sin results are incorrect on complex inputs with small absolute value</t>
+  </si>
+  <si>
+    <t>Did not attempt: mathematical operator specific bug</t>
+  </si>
+  <si>
+    <t>[shmap] shard_map doesn't support multiple axes</t>
+  </si>
+  <si>
+    <t>Did not attempt: data structure specific bug</t>
+  </si>
+  <si>
     <t>log_softmax and softmax are not numerically stable with where argument inside vmap</t>
   </si>
   <si>
@@ -48,6 +90,63 @@
     <t>log_softmax()</t>
   </si>
   <si>
+    <t>shard_alike ignores single-device shardings</t>
+  </si>
+  <si>
+    <t>BUG: shard_alike requires newer jaxlib</t>
+  </si>
+  <si>
+    <t>Concatenation error in jax.numpy.diff</t>
+  </si>
+  <si>
+    <t>Array any and all methods missing where parameter in type signature</t>
+  </si>
+  <si>
+    <t>broadcast_to raise Disallowed host-to-device transfer when used inside jax.jit</t>
+  </si>
+  <si>
+    <t>Unexpected behavior of jax.scipy.stats.binom.pmf</t>
+  </si>
+  <si>
+    <t>Testing __cuda_array_interface__ attribute of a CPU array throws an exception</t>
+  </si>
+  <si>
+    <t>Default lowering pass for lu_p has accuracy issue</t>
+  </si>
+  <si>
+    <t>float() argument TypeError in a scan</t>
+  </si>
+  <si>
+    <t>GPU memory allocation not working as expected</t>
+  </si>
+  <si>
+    <t>jnp.min or jnp.max returns nan if input array dtype is fp8</t>
+  </si>
+  <si>
+    <t>Did not attempt: general operation specific bug</t>
+  </si>
+  <si>
+    <t>[jax_dynamic_shapes] specifying shapes with floating point abstract values does not raise a TypeError</t>
+  </si>
+  <si>
+    <t>JAX hangs when allocating array of at least 2^19 bytes on CPU in subprocess</t>
+  </si>
+  <si>
+    <t>shard_map throws a NotImplementedError: No replication rule for erf_inv</t>
+  </si>
+  <si>
+    <t>debug.print looks strange in jaxpr representation</t>
+  </si>
+  <si>
+    <t>Did not attempt: debug specific bug</t>
+  </si>
+  <si>
+    <t>Add replication rules for convolutions</t>
+  </si>
+  <si>
+    <t>AOT path doesn't typecheck DCE'd arguments</t>
+  </si>
+  <si>
     <t>NaN Error only in combination of disable_jit and debug_nans</t>
   </si>
   <si>
@@ -57,12 +156,88 @@
     <t>_canonicalize_float_for_sort()</t>
   </si>
   <si>
+    <t>Array indexing: boolean mask after newaxis leads to error</t>
+  </si>
+  <si>
+    <t>Template class in extern "C" block causes failure of compilation under MSVC on Windows</t>
+  </si>
+  <si>
+    <t>Large multi-channel inverse FFTs give wrong results</t>
+  </si>
+  <si>
+    <t>Cannot take gradient of VJP function involving new-style RNG key</t>
+  </si>
+  <si>
+    <t>[Pallas] GPU: CUDA error when kernel launch dimensions &gt;= 65536 in Y or Z</t>
+  </si>
+  <si>
+    <t>[jax2tf] InconclusiveDimensionOperation for scatter op with leading vmapped symbolic dimension</t>
+  </si>
+  <si>
+    <t>Repeatedly building JAX causes string substitution failures</t>
+  </si>
+  <si>
+    <t>BCOO.fromdense is not compatible with jax.vmap</t>
+  </si>
+  <si>
+    <t>jnp.linalg.eig errors for invalid inputs instead of returning nan</t>
+  </si>
+  <si>
+    <t>Constant factor error in JAX 101 docs</t>
+  </si>
+  <si>
     <t>PyTreeDef.num_leaves returns the wrong result when composed</t>
   </si>
   <si>
     <t>Force pushed</t>
   </si>
   <si>
+    <t xml:space="preserve">is:issue is:closed created:2024-03-18..2024-03-27 </t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">There is a comment error in </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>test_transformers.py</t>
+    </r>
+  </si>
+  <si>
+    <t>UserWarning when using Tensor Model Parallel libraries (megatron and fairscale)</t>
+  </si>
+  <si>
+    <t>allow storage to be created for ort</t>
+  </si>
+  <si>
+    <t>MPS: Implement index_select() on complex value</t>
+  </si>
+  <si>
+    <t>Mergebot should send a cleaner message when [no ci] message added to the PR commit</t>
+  </si>
+  <si>
+    <t>torch compile item() cannot convert symbols to int error</t>
+  </si>
+  <si>
+    <t>torch/_inductor/compile_fx.py,torch/_inductor/graph.py</t>
+  </si>
+  <si>
+    <t>fx_codegen_and_compile(),run_node()</t>
+  </si>
+  <si>
+    <t>[inductor][cpu] pyhpc_equation_of_state fp32 static shape default/cpp wrapper multiple thread performance test crashed</t>
+  </si>
+  <si>
+    <t>[dort][dynamo_export] Wrong model for phi backward graph</t>
+  </si>
+  <si>
+    <t>[ONNX] Dispatcher does not handle list correctly when the first element is None</t>
+  </si>
+  <si>
     <t>split_with_sizes with unbacked SymInt results in buffers that cannot be materialized for extern calls</t>
   </si>
   <si>
@@ -72,39 +247,21 @@
     <t>SliceView.create(),slice_()</t>
   </si>
   <si>
-    <t>torch compile item() cannot convert symbols to int error</t>
-  </si>
-  <si>
-    <t>torch/_inductor/compile_fx.py,torch/_inductor/graph.py</t>
-  </si>
-  <si>
-    <t>fx_codegen_and_compile(),run_node()</t>
-  </si>
-  <si>
-    <t>Filter:</t>
+    <t>CUDA Being Initiated Early After Importing Certain Libraries on Nightly Build</t>
   </si>
   <si>
     <t xml:space="preserve">is:issue is:closed created:2023-12-01..2024-03-27 label:type:bug </t>
   </si>
   <si>
-    <t>Remarks</t>
-  </si>
-  <si>
     <t>tf.raw_ops.UnravelIndex can leads to eigen assertion failure</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>tensorflow/core/kernels/unravel_index_op.cc</t>
   </si>
   <si>
     <t>UnravelIndexOp.Compute()</t>
   </si>
   <si>
-    <t>Did not reproduce: general operation specific bug</t>
-  </si>
-  <si>
     <t>tf.raw_ops.Substr can lead to eigen assertion failure</t>
   </si>
   <si>
@@ -132,7 +289,7 @@
     <t>PyGraphData.Clear()</t>
   </si>
   <si>
-    <t>Did not reproduce: data structure specific bug</t>
+    <t>Did not attempt: data structure specific bug specific bug</t>
   </si>
   <si>
     <t>tf.raw_ops.DrawBoundingBoxesV2 aborts with inappropriate input</t>
@@ -162,7 +319,7 @@
     <t>Tests</t>
   </si>
   <si>
-    <t>Did not reproduce: fixing tests</t>
+    <t>Did not attempt: fixing tests</t>
   </si>
   <si>
     <t>mkl_remapper_test fails with TF_ENABLE_ONEDNN_OPTS=1</t>
@@ -187,7 +344,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -203,13 +360,23 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <color rgb="FF1F2328"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -218,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -229,6 +396,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -474,9 +644,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="65.5"/>
+    <col customWidth="1" min="3" max="3" width="81.38"/>
     <col customWidth="1" min="6" max="6" width="28.75"/>
     <col customWidth="1" min="7" max="7" width="22.88"/>
+    <col customWidth="1" min="8" max="8" width="40.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -486,168 +657,696 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>19490.0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>19518.0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>18680.0</v>
-      </c>
-      <c r="B3" s="2">
-        <v>18682.0</v>
+        <v>20267.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
+        <v>20135.0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>20082.0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>19992.0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>19978.0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>19753.0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>19663.0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>19490.0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>19518.0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>19459.0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>19440.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <v>19362.0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <v>19356.0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <v>19334.0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2">
+        <v>19150.0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <v>19134.0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2">
+        <v>19076.0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2">
+        <v>19059.0</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2">
+        <v>19035.0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2">
+        <v>19011.0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2">
+        <v>18937.0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2">
+        <v>18852.0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2">
+        <v>18851.0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2">
+        <v>18802.0</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2">
+        <v>18737.0</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2">
+        <v>18686.0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2">
+        <v>18680.0</v>
+      </c>
+      <c r="B28" s="2">
+        <v>18682.0</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2">
+        <v>18542.0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2">
+        <v>18455.0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2">
+        <v>18453.0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2">
+        <v>18442.0</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2">
+        <v>18361.0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2">
+        <v>18348.0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2">
+        <v>18252.0</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2">
+        <v>18245.0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2">
+        <v>18226.0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2">
+        <v>18219.0</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2">
         <v>18218.0</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B39" s="2">
         <v>6501.0</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
+      <c r="C39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Z1000">
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:Z1001">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Force pushed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Z1000">
+  <conditionalFormatting sqref="A1:Z1001">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula> $D1 = "YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="A3"/>
-    <hyperlink r:id="rId4" ref="B3"/>
-    <hyperlink r:id="rId5" ref="A4"/>
-    <hyperlink r:id="rId6" ref="B4"/>
+    <hyperlink r:id="rId1" ref="A3"/>
+    <hyperlink r:id="rId2" ref="A4"/>
+    <hyperlink r:id="rId3" ref="A5"/>
+    <hyperlink r:id="rId4" ref="A6"/>
+    <hyperlink r:id="rId5" ref="A7"/>
+    <hyperlink r:id="rId6" ref="A8"/>
+    <hyperlink r:id="rId7" ref="A9"/>
+    <hyperlink r:id="rId8" ref="A10"/>
+    <hyperlink r:id="rId9" ref="B10"/>
+    <hyperlink r:id="rId10" ref="A11"/>
+    <hyperlink r:id="rId11" ref="A12"/>
+    <hyperlink r:id="rId12" ref="A13"/>
+    <hyperlink r:id="rId13" ref="A14"/>
+    <hyperlink r:id="rId14" ref="A15"/>
+    <hyperlink r:id="rId15" ref="A16"/>
+    <hyperlink r:id="rId16" ref="A17"/>
+    <hyperlink r:id="rId17" ref="A18"/>
+    <hyperlink r:id="rId18" ref="A19"/>
+    <hyperlink r:id="rId19" ref="A20"/>
+    <hyperlink r:id="rId20" ref="A21"/>
+    <hyperlink r:id="rId21" ref="A22"/>
+    <hyperlink r:id="rId22" ref="A23"/>
+    <hyperlink r:id="rId23" ref="A24"/>
+    <hyperlink r:id="rId24" ref="A25"/>
+    <hyperlink r:id="rId25" ref="A26"/>
+    <hyperlink r:id="rId26" ref="A27"/>
+    <hyperlink r:id="rId27" ref="A28"/>
+    <hyperlink r:id="rId28" ref="B28"/>
+    <hyperlink r:id="rId29" ref="A29"/>
+    <hyperlink r:id="rId30" ref="A30"/>
+    <hyperlink r:id="rId31" ref="A31"/>
+    <hyperlink r:id="rId32" ref="A32"/>
+    <hyperlink r:id="rId33" ref="A33"/>
+    <hyperlink r:id="rId34" ref="A34"/>
+    <hyperlink r:id="rId35" ref="A35"/>
+    <hyperlink r:id="rId36" ref="A36"/>
+    <hyperlink r:id="rId37" ref="A37"/>
+    <hyperlink r:id="rId38" ref="A38"/>
+    <hyperlink r:id="rId39" ref="A39"/>
+    <hyperlink r:id="rId40" ref="B39"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId41"/>
 </worksheet>
 </file>
 
@@ -663,7 +1362,7 @@
   <cols>
     <col customWidth="1" min="3" max="3" width="74.13"/>
     <col customWidth="1" min="6" max="6" width="35.88"/>
-    <col customWidth="1" min="7" max="7" width="15.25"/>
+    <col customWidth="1" min="7" max="7" width="31.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -671,126 +1370,275 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>122126.0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>122149.0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
+        <v>122594.0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>122521.0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>122445.0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>122427.0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>122407.0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
         <v>122296.0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B8" s="2">
         <v>122298.0</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
+      <c r="C8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>122283.0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>122181.0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>122166.0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>122126.0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>122149.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <v>122085.0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Z1">
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:Z2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Force pushed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Z1000">
+  <conditionalFormatting sqref="A1:Z1001">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula> $D1 = "YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="A3"/>
-    <hyperlink r:id="rId4" ref="B3"/>
+    <hyperlink r:id="rId1" ref="A3"/>
+    <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
+    <hyperlink r:id="rId4" ref="A5"/>
+    <hyperlink r:id="rId5" ref="A6"/>
+    <hyperlink r:id="rId6" ref="A7"/>
+    <hyperlink r:id="rId7" ref="A8"/>
+    <hyperlink r:id="rId8" ref="B8"/>
+    <hyperlink r:id="rId9" ref="A9"/>
+    <hyperlink r:id="rId10" ref="A10"/>
+    <hyperlink r:id="rId11" ref="A11"/>
+    <hyperlink r:id="rId12" ref="A12"/>
+    <hyperlink r:id="rId13" ref="B12"/>
+    <hyperlink r:id="rId14" ref="A13"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -811,10 +1659,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -824,28 +1672,28 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -856,22 +1704,22 @@
         <v>63092.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
@@ -882,22 +1730,22 @@
         <v>63091.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
@@ -908,22 +1756,22 @@
         <v>63050.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
@@ -934,22 +1782,22 @@
         <v>63083.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7">
@@ -960,22 +1808,22 @@
         <v>63105.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
@@ -986,22 +1834,22 @@
         <v>62990.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
@@ -1012,22 +1860,22 @@
         <v>62897.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10">
@@ -1038,22 +1886,22 @@
         <v>62876.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11">
@@ -1064,22 +1912,22 @@
         <v>7899.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>

</xml_diff>

<commit_message>
Updated the filter in the spreadsheets
</commit_message>
<xml_diff>
--- a/bug_dataset.xlsx
+++ b/bug_dataset.xlsx
@@ -18,7 +18,7 @@
     <t>Filter:</t>
   </si>
   <si>
-    <t>is:issue is:closed created:2023-10-20..2024-03-27 label:bug</t>
+    <t>is:issue is:closed created:2023-10-20..2024-03-27 label:bug linked:pr</t>
   </si>
   <si>
     <t>Issue #</t>
@@ -192,7 +192,7 @@
     <t>Force pushed</t>
   </si>
   <si>
-    <t xml:space="preserve">is:issue is:closed created:2024-03-18..2024-03-27 </t>
+    <t>is:issue is:closed created:2024-03-18..2024-03-27 linked:pr</t>
   </si>
   <si>
     <r>
@@ -250,7 +250,7 @@
     <t>CUDA Being Initiated Early After Importing Certain Libraries on Nightly Build</t>
   </si>
   <si>
-    <t xml:space="preserve">is:issue is:closed created:2023-12-01..2024-03-27 label:type:bug </t>
+    <t>is:issue is:closed created:2023-12-01..2024-03-27 label:type:bug linked:pr</t>
   </si>
   <si>
     <t>tf.raw_ops.UnravelIndex can leads to eigen assertion failure</t>

</xml_diff>

<commit_message>
Updated spreadsheet to remove a redundant column
</commit_message>
<xml_diff>
--- a/bug_dataset.xlsx
+++ b/bug_dataset.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="104">
   <si>
     <t>Filter:</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Reproduced</t>
   </si>
   <si>
-    <t>Fixed</t>
-  </si>
-  <si>
     <t>Buggy File(s)</t>
   </si>
   <si>
@@ -123,7 +120,7 @@
     <t>jnp.min or jnp.max returns nan if input array dtype is fp8</t>
   </si>
   <si>
-    <t>Did not attempt: general operation specific bug</t>
+    <t>Did not attempt: general non-dnn bug</t>
   </si>
   <si>
     <t>[jax_dynamic_shapes] specifying shapes with floating point abstract values does not raise a TypeError</t>
@@ -645,9 +642,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="3" max="3" width="81.38"/>
-    <col customWidth="1" min="6" max="6" width="28.75"/>
-    <col customWidth="1" min="7" max="7" width="22.88"/>
-    <col customWidth="1" min="8" max="8" width="40.38"/>
+    <col customWidth="1" min="5" max="5" width="28.75"/>
+    <col customWidth="1" min="6" max="6" width="22.88"/>
+    <col customWidth="1" min="7" max="7" width="40.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -660,7 +657,6 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -684,22 +680,19 @@
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
         <v>20267.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -707,13 +700,13 @@
         <v>20135.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -721,13 +714,13 @@
         <v>20082.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -735,13 +728,13 @@
         <v>19992.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
@@ -749,13 +742,13 @@
         <v>19978.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -763,13 +756,13 @@
         <v>19753.0</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9">
@@ -777,13 +770,13 @@
         <v>19663.0</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -794,10 +787,10 @@
         <v>19518.0</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>22</v>
@@ -805,9 +798,7 @@
       <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -826,20 +817,19 @@
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="2">
         <v>19459.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -847,13 +837,13 @@
         <v>19440.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13">
@@ -861,13 +851,13 @@
         <v>19362.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14">
@@ -875,13 +865,13 @@
         <v>19356.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -889,13 +879,13 @@
         <v>19334.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16">
@@ -903,13 +893,13 @@
         <v>19150.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17">
@@ -917,13 +907,13 @@
         <v>19134.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18">
@@ -931,13 +921,13 @@
         <v>19076.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19">
@@ -945,13 +935,13 @@
         <v>19059.0</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20">
@@ -959,13 +949,13 @@
         <v>19035.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21">
@@ -973,13 +963,13 @@
         <v>19011.0</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="22">
@@ -987,13 +977,13 @@
         <v>18937.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23">
@@ -1001,13 +991,13 @@
         <v>18852.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24">
@@ -1015,13 +1005,13 @@
         <v>18851.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="25">
@@ -1029,13 +1019,13 @@
         <v>18802.0</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="26">
@@ -1043,13 +1033,13 @@
         <v>18737.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="27">
@@ -1057,13 +1047,13 @@
         <v>18686.0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="28">
@@ -1074,20 +1064,18 @@
         <v>18682.0</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
@@ -1106,20 +1094,19 @@
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
-      <c r="Z28" s="3"/>
     </row>
     <row r="29">
       <c r="A29" s="2">
         <v>18542.0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="30">
@@ -1127,13 +1114,13 @@
         <v>18455.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="31">
@@ -1141,13 +1128,13 @@
         <v>18453.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="32">
@@ -1155,13 +1142,13 @@
         <v>18442.0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="33">
@@ -1169,13 +1156,13 @@
         <v>18361.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="34">
@@ -1183,13 +1170,13 @@
         <v>18348.0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="35">
@@ -1197,13 +1184,13 @@
         <v>18252.0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="36">
@@ -1211,13 +1198,13 @@
         <v>18245.0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="37">
@@ -1225,13 +1212,13 @@
         <v>18226.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="38">
@@ -1239,13 +1226,13 @@
         <v>18219.0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="39">
@@ -1256,20 +1243,18 @@
         <v>6501.0</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F39" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
@@ -1288,18 +1273,17 @@
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
       <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:Z1001">
+  <conditionalFormatting sqref="A1:Y1001">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Force pushed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Z1001">
+  <conditionalFormatting sqref="A1:Y1001">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula> $D1 = "YES"</formula>
     </cfRule>
@@ -1361,8 +1345,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="3" max="3" width="74.13"/>
-    <col customWidth="1" min="6" max="6" width="35.88"/>
-    <col customWidth="1" min="7" max="7" width="31.75"/>
+    <col customWidth="1" min="5" max="5" width="35.88"/>
+    <col customWidth="1" min="6" max="6" width="31.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1370,13 +1354,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -1400,22 +1383,19 @@
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
         <v>122594.0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -1423,13 +1403,13 @@
         <v>122521.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -1437,13 +1417,13 @@
         <v>122445.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -1451,13 +1431,13 @@
         <v>122427.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
@@ -1465,13 +1445,13 @@
         <v>122407.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8">
@@ -1482,20 +1462,18 @@
         <v>122298.0</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -1514,20 +1492,19 @@
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="2">
         <v>122283.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -1535,13 +1512,13 @@
         <v>122181.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11">
@@ -1549,13 +1526,13 @@
         <v>122166.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12">
@@ -1566,20 +1543,18 @@
         <v>122149.0</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1598,26 +1573,25 @@
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" s="2">
         <v>122085.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:Z2">
+  <conditionalFormatting sqref="A1:Y2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Force pushed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Z1001">
+  <conditionalFormatting sqref="A1:Y1001">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula> $D1 = "YES"</formula>
     </cfRule>
@@ -1653,8 +1627,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="3" max="3" width="76.38"/>
-    <col customWidth="1" min="7" max="7" width="24.38"/>
-    <col customWidth="1" min="8" max="8" width="47.75"/>
+    <col customWidth="1" min="6" max="6" width="24.38"/>
+    <col customWidth="1" min="7" max="7" width="47.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1662,13 +1636,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -1692,9 +1665,6 @@
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
@@ -1704,22 +1674,19 @@
         <v>63092.0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>77</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
@@ -1730,22 +1697,19 @@
         <v>63091.0</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>80</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
@@ -1756,22 +1720,19 @@
         <v>63050.0</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>83</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6">
@@ -1782,22 +1743,19 @@
         <v>63083.0</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>86</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="7">
@@ -1808,22 +1766,19 @@
         <v>63105.0</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>90</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
@@ -1834,22 +1789,19 @@
         <v>62990.0</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>93</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -1860,22 +1812,19 @@
         <v>62897.0</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>96</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="10">
@@ -1886,22 +1835,19 @@
         <v>62876.0</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="11">
@@ -1912,23 +1858,21 @@
         <v>7899.0</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>102</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1946,18 +1890,17 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:Z2">
+  <conditionalFormatting sqref="A1:Y2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Force pushed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:Z1001">
+  <conditionalFormatting sqref="A1:Y1001">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula> $D1 = "YES"</formula>
     </cfRule>
@@ -1981,7 +1924,7 @@
     <hyperlink r:id="rId16" ref="B10"/>
     <hyperlink r:id="rId17" ref="A11"/>
     <hyperlink r:id="rId18" ref="B11"/>
-    <hyperlink r:id="rId19" ref="F11"/>
+    <hyperlink r:id="rId19" ref="E11"/>
   </hyperlinks>
   <drawing r:id="rId20"/>
 </worksheet>

</xml_diff>

<commit_message>
Added sperate CSV files for each library
</commit_message>
<xml_diff>
--- a/bug_dataset.xlsx
+++ b/bug_dataset.xlsx
@@ -648,13 +648,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
@@ -1276,7 +1275,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:Y1001">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -1350,13 +1349,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1584,7 +1582,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:Y2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -1632,13 +1630,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1893,7 +1890,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:Y2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>